<commit_message>
Add results on other resolutions, add algorithm steps in RO and conclusions
</commit_message>
<xml_diff>
--- a/ResultsTable.xlsx
+++ b/ResultsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1Proiecte\MATLAB-Python-Facultate\PAIC Proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2253C152-4B65-4A5E-890E-97E3FB540F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7D1538-A0D8-471A-A457-3BCDF76ABA88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
   <si>
     <t>Filter</t>
   </si>
@@ -65,6 +65,129 @@
   </si>
   <si>
     <t>Image / Filter</t>
+  </si>
+  <si>
+    <t>lena_color_256</t>
+  </si>
+  <si>
+    <t>peppers_256</t>
+  </si>
+  <si>
+    <t>penguins_256</t>
+  </si>
+  <si>
+    <t>baboon_256</t>
+  </si>
+  <si>
+    <t>lighthouse_256</t>
+  </si>
+  <si>
+    <t>parrots_256</t>
+  </si>
+  <si>
+    <t>lena_color_128</t>
+  </si>
+  <si>
+    <t>peppers_128</t>
+  </si>
+  <si>
+    <t>penguins_128</t>
+  </si>
+  <si>
+    <t>baboon_128</t>
+  </si>
+  <si>
+    <t>lighthouse_128</t>
+  </si>
+  <si>
+    <t>parrots_128</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.31s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.87s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.29s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.54s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.27s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.07s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.96s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.30s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.33s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.67s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.34s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.18s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.12s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.04s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.26s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.05s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.25s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">64.51s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.09s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.19s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.46s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">64.08s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.20s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.47s  </t>
   </si>
 </sst>
 </file>
@@ -382,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +721,574 @@
       </c>
       <c r="E13">
         <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>27.931000000000001</v>
+      </c>
+      <c r="D17">
+        <v>29.771999999999998</v>
+      </c>
+      <c r="E17">
+        <v>28.521000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>4.0220000000000002</v>
+      </c>
+      <c r="D18">
+        <v>1.601</v>
+      </c>
+      <c r="E18">
+        <v>2.3170000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>28.052</v>
+      </c>
+      <c r="D20">
+        <v>29.350999999999999</v>
+      </c>
+      <c r="E20">
+        <v>28.555</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>3.161</v>
+      </c>
+      <c r="D21">
+        <v>1.329</v>
+      </c>
+      <c r="E21">
+        <v>1.714</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>26.626999999999999</v>
+      </c>
+      <c r="D23">
+        <v>28.64</v>
+      </c>
+      <c r="E23">
+        <v>27.07</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>3.8220000000000001</v>
+      </c>
+      <c r="D24">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="E24">
+        <v>2.5510000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>23.026</v>
+      </c>
+      <c r="D26">
+        <v>26.073</v>
+      </c>
+      <c r="E26">
+        <v>23.728999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>10.744999999999999</v>
+      </c>
+      <c r="D27">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="E27">
+        <v>7.5839999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>25.699000000000002</v>
+      </c>
+      <c r="D29">
+        <v>27.478999999999999</v>
+      </c>
+      <c r="E29">
+        <v>26.265999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>5.5620000000000003</v>
+      </c>
+      <c r="D30">
+        <v>2.3530000000000002</v>
+      </c>
+      <c r="E30">
+        <v>3.7149999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>28.875</v>
+      </c>
+      <c r="D32">
+        <v>30.422000000000001</v>
+      </c>
+      <c r="E32">
+        <v>29.248999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>2.4</v>
+      </c>
+      <c r="D33">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="E33">
+        <v>1.4119999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>26.113</v>
+      </c>
+      <c r="D39">
+        <v>27.49</v>
+      </c>
+      <c r="E39">
+        <v>26.472999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>4.2590000000000003</v>
+      </c>
+      <c r="D40">
+        <v>1.79</v>
+      </c>
+      <c r="E40">
+        <v>2.7160000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>25.202999999999999</v>
+      </c>
+      <c r="D42">
+        <v>26.901</v>
+      </c>
+      <c r="E42">
+        <v>25.63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>4.3360000000000003</v>
+      </c>
+      <c r="D43">
+        <v>1.734</v>
+      </c>
+      <c r="E43">
+        <v>1.734</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>24.306000000000001</v>
+      </c>
+      <c r="D45">
+        <v>26.353000000000002</v>
+      </c>
+      <c r="E45">
+        <v>24.658999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>5.0919999999999996</v>
+      </c>
+      <c r="D46">
+        <v>2.1240000000000001</v>
+      </c>
+      <c r="E46">
+        <v>3.5590000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>23.896000000000001</v>
+      </c>
+      <c r="D48">
+        <v>26.077000000000002</v>
+      </c>
+      <c r="E48">
+        <v>24.58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>8.9879999999999995</v>
+      </c>
+      <c r="D49">
+        <v>3.46</v>
+      </c>
+      <c r="E49">
+        <v>6.1210000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>25.146999999999998</v>
+      </c>
+      <c r="D51">
+        <v>26.814</v>
+      </c>
+      <c r="E51">
+        <v>25.684999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>5.5839999999999996</v>
+      </c>
+      <c r="D52">
+        <v>2.371</v>
+      </c>
+      <c r="E52">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>26.291</v>
+      </c>
+      <c r="D54">
+        <v>27.382999999999999</v>
+      </c>
+      <c r="E54">
+        <v>26.619</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>3.3980000000000001</v>
+      </c>
+      <c r="D55">
+        <v>1.4590000000000001</v>
+      </c>
+      <c r="E55">
+        <v>2.1349999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>